<commit_message>
Se rehizo la matriz sin redundancias, luego de cambiar algunas presedencias de forma manual en la matriz original
</commit_message>
<xml_diff>
--- a/Modelo/Códigos para matriz/matriz_sin_redundancia.xlsx
+++ b/Modelo/Códigos para matriz/matriz_sin_redundancia.xlsx
@@ -707,7 +707,7 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -716,7 +716,7 @@
         <v>1</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -912,10 +912,10 @@
         <v>0</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -1114,7 +1114,7 @@
         <v>0</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -1126,7 +1126,7 @@
         <v>1</v>
       </c>
       <c r="G4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H4">
         <v>1</v>
@@ -1319,7 +1319,7 @@
         <v>0</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -1732,7 +1732,7 @@
         <v>0</v>
       </c>
       <c r="D7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E7">
         <v>0</v>
@@ -2769,7 +2769,7 @@
         <v>0</v>
       </c>
       <c r="H12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I12">
         <v>1</v>
@@ -2959,7 +2959,7 @@
         <v>0</v>
       </c>
       <c r="C13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D13">
         <v>0</v>

</xml_diff>

<commit_message>
Modificaciones en la matriz (sin redundancias, para esto se eliminaron las doble dependencia de algunos conceptos), documentos a revisar por la SP y se agrega planilla de juicio de expertos, se modificó la presentación para SP
</commit_message>
<xml_diff>
--- a/Modelo/Códigos para matriz/matriz_sin_redundancia.xlsx
+++ b/Modelo/Códigos para matriz/matriz_sin_redundancia.xlsx
@@ -722,46 +722,46 @@
         <v>0</v>
       </c>
       <c r="I2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J2">
         <v>1</v>
       </c>
       <c r="K2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P2">
         <v>0</v>
       </c>
       <c r="Q2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S2">
         <v>0</v>
       </c>
       <c r="T2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W2">
         <v>0</v>
@@ -770,7 +770,7 @@
         <v>0</v>
       </c>
       <c r="Y2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z2">
         <v>0</v>
@@ -779,10 +779,10 @@
         <v>0</v>
       </c>
       <c r="AB2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD2">
         <v>0</v>
@@ -791,70 +791,70 @@
         <v>0</v>
       </c>
       <c r="AF2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AM2">
         <v>0</v>
       </c>
       <c r="AN2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AO2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AP2">
         <v>0</v>
       </c>
       <c r="AQ2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AR2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AS2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AT2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AU2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AV2">
         <v>0</v>
       </c>
       <c r="AW2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AX2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AY2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AZ2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BA2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BB2">
         <v>0</v>
@@ -863,16 +863,16 @@
         <v>0</v>
       </c>
       <c r="BD2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BE2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BF2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BG2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BH2">
         <v>0</v>
@@ -881,19 +881,19 @@
         <v>0</v>
       </c>
       <c r="BJ2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BK2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BL2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BM2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BN2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BO2">
         <v>0</v>
@@ -1129,25 +1129,25 @@
         <v>1</v>
       </c>
       <c r="H4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J4">
         <v>1</v>
       </c>
       <c r="K4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L4">
         <v>0</v>
       </c>
       <c r="M4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O4">
         <v>0</v>
@@ -1168,25 +1168,25 @@
         <v>0</v>
       </c>
       <c r="U4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W4">
         <v>0</v>
       </c>
       <c r="X4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z4">
         <v>0</v>
       </c>
       <c r="AA4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB4">
         <v>0</v>
@@ -1201,7 +1201,7 @@
         <v>0</v>
       </c>
       <c r="AF4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG4">
         <v>0</v>
@@ -1225,7 +1225,7 @@
         <v>0</v>
       </c>
       <c r="AN4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AO4">
         <v>0</v>
@@ -1234,16 +1234,16 @@
         <v>0</v>
       </c>
       <c r="AQ4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AR4">
         <v>0</v>
       </c>
       <c r="AS4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AT4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AU4">
         <v>0</v>
@@ -1252,7 +1252,7 @@
         <v>0</v>
       </c>
       <c r="AW4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AX4">
         <v>0</v>
@@ -1276,7 +1276,7 @@
         <v>0</v>
       </c>
       <c r="BE4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BF4">
         <v>0</v>
@@ -1297,7 +1297,7 @@
         <v>0</v>
       </c>
       <c r="BL4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BM4">
         <v>0</v>
@@ -1349,10 +1349,10 @@
         <v>0</v>
       </c>
       <c r="M5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O5">
         <v>0</v>
@@ -1361,10 +1361,10 @@
         <v>0</v>
       </c>
       <c r="Q5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S5">
         <v>0</v>
@@ -1376,16 +1376,16 @@
         <v>0</v>
       </c>
       <c r="V5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W5">
         <v>0</v>
       </c>
       <c r="X5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z5">
         <v>0</v>
@@ -1406,7 +1406,7 @@
         <v>0</v>
       </c>
       <c r="AF5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG5">
         <v>1</v>
@@ -1415,7 +1415,7 @@
         <v>0</v>
       </c>
       <c r="AI5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ5">
         <v>0</v>
@@ -1439,16 +1439,16 @@
         <v>0</v>
       </c>
       <c r="AQ5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AR5">
         <v>0</v>
       </c>
       <c r="AS5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AT5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AU5">
         <v>0</v>
@@ -1457,7 +1457,7 @@
         <v>0</v>
       </c>
       <c r="AW5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AX5">
         <v>0</v>
@@ -1505,7 +1505,7 @@
         <v>0</v>
       </c>
       <c r="BM5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BN5">
         <v>0</v>
@@ -1554,7 +1554,7 @@
         <v>0</v>
       </c>
       <c r="M6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N6">
         <v>0</v>
@@ -1602,7 +1602,7 @@
         <v>0</v>
       </c>
       <c r="AC6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD6">
         <v>0</v>
@@ -1611,7 +1611,7 @@
         <v>0</v>
       </c>
       <c r="AF6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG6">
         <v>0</v>
@@ -1650,7 +1650,7 @@
         <v>0</v>
       </c>
       <c r="AS6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AT6">
         <v>0</v>
@@ -1722,7 +1722,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Cotizaciones_previsionales</t>
+          <t>Cotizaciones_Previsionales</t>
         </is>
       </c>
       <c r="B7">
@@ -1747,16 +1747,16 @@
         <v>1</v>
       </c>
       <c r="I7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J7">
         <v>0</v>
       </c>
       <c r="K7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M7">
         <v>0</v>
@@ -1792,7 +1792,7 @@
         <v>0</v>
       </c>
       <c r="X7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y7">
         <v>0</v>
@@ -1819,7 +1819,7 @@
         <v>0</v>
       </c>
       <c r="AG7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH7">
         <v>0</v>
@@ -1840,7 +1840,7 @@
         <v>0</v>
       </c>
       <c r="AN7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AO7">
         <v>0</v>
@@ -1849,13 +1849,13 @@
         <v>0</v>
       </c>
       <c r="AQ7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AR7">
         <v>0</v>
       </c>
       <c r="AS7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AT7">
         <v>0</v>
@@ -1867,7 +1867,7 @@
         <v>0</v>
       </c>
       <c r="AW7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AX7">
         <v>0</v>
@@ -1879,7 +1879,7 @@
         <v>0</v>
       </c>
       <c r="BA7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BB7">
         <v>0</v>
@@ -1888,13 +1888,13 @@
         <v>0</v>
       </c>
       <c r="BD7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BE7">
         <v>0</v>
       </c>
       <c r="BF7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BG7">
         <v>0</v>
@@ -1952,19 +1952,19 @@
         <v>0</v>
       </c>
       <c r="I8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J8">
         <v>0</v>
       </c>
       <c r="K8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N8">
         <v>0</v>
@@ -1997,7 +1997,7 @@
         <v>0</v>
       </c>
       <c r="X8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y8">
         <v>0</v>
@@ -2015,19 +2015,19 @@
         <v>0</v>
       </c>
       <c r="AD8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG8">
         <v>1</v>
       </c>
       <c r="AH8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI8">
         <v>0</v>
@@ -2042,34 +2042,34 @@
         <v>0</v>
       </c>
       <c r="AM8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN8">
         <v>1</v>
       </c>
       <c r="AO8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AP8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AQ8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AR8">
         <v>0</v>
       </c>
       <c r="AS8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AT8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AU8">
         <v>0</v>
       </c>
       <c r="AV8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AW8">
         <v>0</v>
@@ -2078,19 +2078,19 @@
         <v>0</v>
       </c>
       <c r="AY8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AZ8">
         <v>0</v>
       </c>
       <c r="BA8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BB8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BC8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BD8">
         <v>0</v>
@@ -2108,7 +2108,7 @@
         <v>0</v>
       </c>
       <c r="BI8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BJ8">
         <v>0</v>
@@ -2166,10 +2166,10 @@
         <v>0</v>
       </c>
       <c r="L9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N9">
         <v>0</v>
@@ -2205,10 +2205,10 @@
         <v>0</v>
       </c>
       <c r="Y9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA9">
         <v>0</v>
@@ -2772,7 +2772,7 @@
         <v>0</v>
       </c>
       <c r="I12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J12">
         <v>0</v>
@@ -2826,7 +2826,7 @@
         <v>0</v>
       </c>
       <c r="AA12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB12">
         <v>0</v>
@@ -2841,7 +2841,7 @@
         <v>0</v>
       </c>
       <c r="AF12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG12">
         <v>0</v>
@@ -2886,7 +2886,7 @@
         <v>0</v>
       </c>
       <c r="AU12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AV12">
         <v>0</v>
@@ -2977,7 +2977,7 @@
         <v>0</v>
       </c>
       <c r="I13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J13">
         <v>0</v>
@@ -2986,22 +2986,22 @@
         <v>0</v>
       </c>
       <c r="L13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M13">
         <v>0</v>
       </c>
       <c r="N13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R13">
         <v>0</v>
@@ -3019,7 +3019,7 @@
         <v>0</v>
       </c>
       <c r="W13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X13">
         <v>0</v>
@@ -3031,7 +3031,7 @@
         <v>0</v>
       </c>
       <c r="AA13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB13">
         <v>0</v>
@@ -3046,7 +3046,7 @@
         <v>0</v>
       </c>
       <c r="AF13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG13">
         <v>0</v>
@@ -3194,13 +3194,13 @@
         <v>0</v>
       </c>
       <c r="M14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N14">
         <v>0</v>
       </c>
       <c r="O14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P14">
         <v>0</v>
@@ -3215,7 +3215,7 @@
         <v>0</v>
       </c>
       <c r="T14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U14">
         <v>0</v>
@@ -3233,7 +3233,7 @@
         <v>0</v>
       </c>
       <c r="Z14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA14">
         <v>0</v>
@@ -3347,7 +3347,7 @@
         <v>0</v>
       </c>
       <c r="BL14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BM14">
         <v>0</v>
@@ -3411,22 +3411,22 @@
         <v>0</v>
       </c>
       <c r="Q15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W15">
         <v>0</v>
@@ -3441,7 +3441,7 @@
         <v>0</v>
       </c>
       <c r="AA15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB15">
         <v>0</v>
@@ -3567,7 +3567,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Opciones_Post_oferta</t>
+          <t>Opciones_Post_Oferta</t>
         </is>
       </c>
       <c r="B16">
@@ -3836,7 +3836,7 @@
         <v>1</v>
       </c>
       <c r="V17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W17">
         <v>1</v>
@@ -4451,7 +4451,7 @@
         <v>1</v>
       </c>
       <c r="V20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W20">
         <v>1</v>
@@ -5898,7 +5898,7 @@
         <v>0</v>
       </c>
       <c r="Z27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA27">
         <v>0</v>
@@ -6052,7 +6052,7 @@
         <v>0</v>
       </c>
       <c r="I28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J28">
         <v>0</v>
@@ -6064,13 +6064,13 @@
         <v>0</v>
       </c>
       <c r="M28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P28">
         <v>0</v>
@@ -6082,7 +6082,7 @@
         <v>0</v>
       </c>
       <c r="S28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T28">
         <v>0</v>
@@ -6100,7 +6100,7 @@
         <v>0</v>
       </c>
       <c r="Y28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z28">
         <v>0</v>
@@ -6112,7 +6112,7 @@
         <v>0</v>
       </c>
       <c r="AC28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD28">
         <v>0</v>
@@ -6121,7 +6121,7 @@
         <v>0</v>
       </c>
       <c r="AF28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG28">
         <v>0</v>
@@ -6220,7 +6220,7 @@
         <v>0</v>
       </c>
       <c r="BM28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BN28">
         <v>0</v>
@@ -6272,10 +6272,10 @@
         <v>1</v>
       </c>
       <c r="N29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P29">
         <v>0</v>
@@ -6326,7 +6326,7 @@
         <v>0</v>
       </c>
       <c r="AF29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG29">
         <v>0</v>
@@ -6365,7 +6365,7 @@
         <v>0</v>
       </c>
       <c r="AS29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AT29">
         <v>0</v>
@@ -6579,7 +6579,7 @@
         <v>0</v>
       </c>
       <c r="AV30">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AW30">
         <v>0</v>
@@ -6784,7 +6784,7 @@
         <v>0</v>
       </c>
       <c r="AV31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AW31">
         <v>0</v>
@@ -7089,13 +7089,13 @@
         <v>0</v>
       </c>
       <c r="M33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P33">
         <v>0</v>
@@ -7104,10 +7104,10 @@
         <v>0</v>
       </c>
       <c r="R33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T33">
         <v>0</v>
@@ -7137,7 +7137,7 @@
         <v>0</v>
       </c>
       <c r="AC33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD33">
         <v>1</v>
@@ -7146,28 +7146,28 @@
         <v>1</v>
       </c>
       <c r="AF33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG33">
         <v>0</v>
       </c>
       <c r="AH33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AM33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN33">
         <v>0</v>
@@ -7182,22 +7182,22 @@
         <v>1</v>
       </c>
       <c r="AR33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AS33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AT33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AU33">
         <v>0</v>
       </c>
       <c r="AV33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AW33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AX33">
         <v>0</v>
@@ -7206,10 +7206,10 @@
         <v>1</v>
       </c>
       <c r="AZ33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BA33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BB33">
         <v>0</v>
@@ -7236,7 +7236,7 @@
         <v>0</v>
       </c>
       <c r="BJ33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BK33">
         <v>0</v>
@@ -7245,7 +7245,7 @@
         <v>0</v>
       </c>
       <c r="BM33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BN33">
         <v>0</v>
@@ -7342,7 +7342,7 @@
         <v>0</v>
       </c>
       <c r="AC34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD34">
         <v>0</v>
@@ -7351,7 +7351,7 @@
         <v>0</v>
       </c>
       <c r="AF34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG34">
         <v>0</v>
@@ -7390,7 +7390,7 @@
         <v>0</v>
       </c>
       <c r="AS34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AT34">
         <v>0</v>
@@ -7499,13 +7499,13 @@
         <v>0</v>
       </c>
       <c r="M35">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N35">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O35">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P35">
         <v>0</v>
@@ -7514,10 +7514,10 @@
         <v>0</v>
       </c>
       <c r="R35">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S35">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T35">
         <v>0</v>
@@ -7547,7 +7547,7 @@
         <v>0</v>
       </c>
       <c r="AC35">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD35">
         <v>0</v>
@@ -7577,7 +7577,7 @@
         <v>1</v>
       </c>
       <c r="AM35">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN35">
         <v>0</v>
@@ -7598,22 +7598,22 @@
         <v>0</v>
       </c>
       <c r="AT35">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AU35">
         <v>0</v>
       </c>
       <c r="AV35">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AW35">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AX35">
         <v>0</v>
       </c>
       <c r="AY35">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AZ35">
         <v>0</v>
@@ -7704,13 +7704,13 @@
         <v>0</v>
       </c>
       <c r="M36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N36">
         <v>0</v>
       </c>
       <c r="O36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P36">
         <v>0</v>
@@ -7809,16 +7809,16 @@
         <v>0</v>
       </c>
       <c r="AV36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AW36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AX36">
         <v>0</v>
       </c>
       <c r="AY36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AZ36">
         <v>0</v>
@@ -7909,13 +7909,13 @@
         <v>0</v>
       </c>
       <c r="M37">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N37">
         <v>0</v>
       </c>
       <c r="O37">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P37">
         <v>0</v>
@@ -8014,16 +8014,16 @@
         <v>0</v>
       </c>
       <c r="AV37">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AW37">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AX37">
         <v>0</v>
       </c>
       <c r="AY37">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AZ37">
         <v>0</v>
@@ -8114,13 +8114,13 @@
         <v>0</v>
       </c>
       <c r="M38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N38">
         <v>0</v>
       </c>
       <c r="O38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P38">
         <v>0</v>
@@ -8219,7 +8219,7 @@
         <v>0</v>
       </c>
       <c r="AV38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AW38">
         <v>0</v>
@@ -8337,7 +8337,7 @@
         <v>0</v>
       </c>
       <c r="S39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T39">
         <v>0</v>
@@ -8367,16 +8367,16 @@
         <v>0</v>
       </c>
       <c r="AC39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE39">
         <v>0</v>
       </c>
       <c r="AF39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG39">
         <v>0</v>
@@ -8424,7 +8424,7 @@
         <v>0</v>
       </c>
       <c r="AV39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AW39">
         <v>0</v>
@@ -8524,13 +8524,13 @@
         <v>0</v>
       </c>
       <c r="M40">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N40">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O40">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P40">
         <v>0</v>
@@ -8542,7 +8542,7 @@
         <v>0</v>
       </c>
       <c r="S40">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T40">
         <v>0</v>
@@ -8572,7 +8572,7 @@
         <v>0</v>
       </c>
       <c r="AC40">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD40">
         <v>1</v>
@@ -8581,7 +8581,7 @@
         <v>1</v>
       </c>
       <c r="AF40">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG40">
         <v>0</v>
@@ -8608,31 +8608,31 @@
         <v>0</v>
       </c>
       <c r="AO40">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AP40">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AQ40">
         <v>1</v>
       </c>
       <c r="AR40">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AS40">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AT40">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AU40">
         <v>0</v>
       </c>
       <c r="AV40">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AW40">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AX40">
         <v>0</v>
@@ -8641,10 +8641,10 @@
         <v>1</v>
       </c>
       <c r="AZ40">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BA40">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BB40">
         <v>0</v>
@@ -8671,13 +8671,13 @@
         <v>0</v>
       </c>
       <c r="BJ40">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BK40">
         <v>0</v>
       </c>
       <c r="BL40">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BM40">
         <v>0</v>
@@ -8777,7 +8777,7 @@
         <v>0</v>
       </c>
       <c r="AC41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD41">
         <v>0</v>
@@ -8786,7 +8786,7 @@
         <v>0</v>
       </c>
       <c r="AF41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG41">
         <v>0</v>
@@ -8825,7 +8825,7 @@
         <v>0</v>
       </c>
       <c r="AS41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AT41">
         <v>0</v>
@@ -8952,7 +8952,7 @@
         <v>0</v>
       </c>
       <c r="S42">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T42">
         <v>0</v>
@@ -8982,16 +8982,16 @@
         <v>0</v>
       </c>
       <c r="AC42">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD42">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE42">
         <v>0</v>
       </c>
       <c r="AF42">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG42">
         <v>0</v>
@@ -9039,7 +9039,7 @@
         <v>0</v>
       </c>
       <c r="AV42">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AW42">
         <v>0</v>
@@ -9139,13 +9139,13 @@
         <v>0</v>
       </c>
       <c r="M43">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N43">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O43">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P43">
         <v>0</v>
@@ -9154,10 +9154,10 @@
         <v>0</v>
       </c>
       <c r="R43">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S43">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T43">
         <v>0</v>
@@ -9187,7 +9187,7 @@
         <v>0</v>
       </c>
       <c r="AC43">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD43">
         <v>0</v>
@@ -9196,7 +9196,7 @@
         <v>0</v>
       </c>
       <c r="AF43">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG43">
         <v>0</v>
@@ -9244,7 +9244,7 @@
         <v>0</v>
       </c>
       <c r="AV43">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AW43">
         <v>0</v>
@@ -9256,10 +9256,10 @@
         <v>0</v>
       </c>
       <c r="AZ43">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BA43">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BB43">
         <v>0</v>
@@ -9286,16 +9286,16 @@
         <v>0</v>
       </c>
       <c r="BJ43">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BK43">
         <v>0</v>
       </c>
       <c r="BL43">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BM43">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BN43">
         <v>0</v>
@@ -9549,13 +9549,13 @@
         <v>0</v>
       </c>
       <c r="M45">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N45">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O45">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P45">
         <v>0</v>
@@ -9564,10 +9564,10 @@
         <v>0</v>
       </c>
       <c r="R45">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S45">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T45">
         <v>0</v>
@@ -9597,7 +9597,7 @@
         <v>0</v>
       </c>
       <c r="AC45">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD45">
         <v>0</v>
@@ -9606,7 +9606,7 @@
         <v>0</v>
       </c>
       <c r="AF45">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG45">
         <v>0</v>
@@ -9651,13 +9651,13 @@
         <v>1</v>
       </c>
       <c r="AU45">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AV45">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AW45">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AX45">
         <v>0</v>
@@ -9702,7 +9702,7 @@
         <v>0</v>
       </c>
       <c r="BL45">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BM45">
         <v>1</v>
@@ -9754,13 +9754,13 @@
         <v>0</v>
       </c>
       <c r="M46">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N46">
         <v>0</v>
       </c>
       <c r="O46">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P46">
         <v>0</v>
@@ -9772,7 +9772,7 @@
         <v>0</v>
       </c>
       <c r="S46">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T46">
         <v>0</v>
@@ -9802,7 +9802,7 @@
         <v>0</v>
       </c>
       <c r="AC46">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD46">
         <v>0</v>
@@ -9859,7 +9859,7 @@
         <v>0</v>
       </c>
       <c r="AV46">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AW46">
         <v>0</v>
@@ -10016,7 +10016,7 @@
         <v>0</v>
       </c>
       <c r="AF47">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG47">
         <v>0</v>
@@ -10055,7 +10055,7 @@
         <v>0</v>
       </c>
       <c r="AS47">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AT47">
         <v>0</v>
@@ -10182,7 +10182,7 @@
         <v>0</v>
       </c>
       <c r="S48">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T48">
         <v>0</v>
@@ -10221,7 +10221,7 @@
         <v>0</v>
       </c>
       <c r="AF48">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG48">
         <v>0</v>
@@ -10366,13 +10366,13 @@
         <v>0</v>
       </c>
       <c r="L49">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M49">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N49">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O49">
         <v>0</v>
@@ -10417,7 +10417,7 @@
         <v>0</v>
       </c>
       <c r="AC49">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD49">
         <v>0</v>
@@ -10438,16 +10438,16 @@
         <v>1</v>
       </c>
       <c r="AJ49">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK49">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL49">
         <v>0</v>
       </c>
       <c r="AM49">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN49">
         <v>0</v>
@@ -10465,7 +10465,7 @@
         <v>0</v>
       </c>
       <c r="AS49">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AT49">
         <v>0</v>
@@ -10474,7 +10474,7 @@
         <v>0</v>
       </c>
       <c r="AV49">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AW49">
         <v>0</v>
@@ -10483,16 +10483,16 @@
         <v>1</v>
       </c>
       <c r="AY49">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AZ49">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BA49">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BB49">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BC49">
         <v>0</v>
@@ -10779,7 +10779,7 @@
         <v>0</v>
       </c>
       <c r="M51">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N51">
         <v>0</v>
@@ -10827,7 +10827,7 @@
         <v>0</v>
       </c>
       <c r="AC51">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD51">
         <v>0</v>
@@ -10845,19 +10845,19 @@
         <v>0</v>
       </c>
       <c r="AI51">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ51">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK51">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL51">
         <v>0</v>
       </c>
       <c r="AM51">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN51">
         <v>0</v>
@@ -10866,7 +10866,7 @@
         <v>0</v>
       </c>
       <c r="AP51">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AQ51">
         <v>0</v>
@@ -10875,7 +10875,7 @@
         <v>0</v>
       </c>
       <c r="AS51">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AT51">
         <v>0</v>
@@ -10884,25 +10884,25 @@
         <v>0</v>
       </c>
       <c r="AV51">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AW51">
         <v>1</v>
       </c>
       <c r="AX51">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AY51">
         <v>0</v>
       </c>
       <c r="AZ51">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BA51">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BB51">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BC51">
         <v>0</v>
@@ -11315,7 +11315,7 @@
         <v>1</v>
       </c>
       <c r="BC53">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BD53">
         <v>0</v>
@@ -11801,10 +11801,10 @@
         <v>0</v>
       </c>
       <c r="L56">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M56">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N56">
         <v>0</v>
@@ -11936,7 +11936,7 @@
         <v>0</v>
       </c>
       <c r="BE56">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BF56">
         <v>0</v>
@@ -12352,7 +12352,7 @@
         <v>0</v>
       </c>
       <c r="BG58">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BH58">
         <v>1</v>
@@ -12361,7 +12361,7 @@
         <v>1</v>
       </c>
       <c r="BJ58">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BK58">
         <v>0</v>
@@ -13462,7 +13462,7 @@
         <v>0</v>
       </c>
       <c r="S64">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T64">
         <v>0</v>
@@ -13492,7 +13492,7 @@
         <v>0</v>
       </c>
       <c r="AC64">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD64">
         <v>0</v>
@@ -13501,7 +13501,7 @@
         <v>0</v>
       </c>
       <c r="AF64">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG64">
         <v>0</v>
@@ -13594,7 +13594,7 @@
         <v>0</v>
       </c>
       <c r="BK64">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BL64">
         <v>0</v>
@@ -13603,10 +13603,10 @@
         <v>0</v>
       </c>
       <c r="BN64">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BO64">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="65">
@@ -13667,7 +13667,7 @@
         <v>0</v>
       </c>
       <c r="S65">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T65">
         <v>0</v>
@@ -13697,7 +13697,7 @@
         <v>0</v>
       </c>
       <c r="AC65">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD65">
         <v>0</v>
@@ -13706,7 +13706,7 @@
         <v>0</v>
       </c>
       <c r="AF65">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG65">
         <v>0</v>
@@ -13799,7 +13799,7 @@
         <v>0</v>
       </c>
       <c r="BK65">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BL65">
         <v>0</v>
@@ -13808,10 +13808,10 @@
         <v>0</v>
       </c>
       <c r="BN65">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BO65">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="66">
@@ -13872,7 +13872,7 @@
         <v>0</v>
       </c>
       <c r="S66">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T66">
         <v>0</v>
@@ -14004,7 +14004,7 @@
         <v>0</v>
       </c>
       <c r="BK66">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BL66">
         <v>0</v>
@@ -14016,7 +14016,7 @@
         <v>0</v>
       </c>
       <c r="BO66">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="67">

</xml_diff>